<commit_message>
addind P21 groups and outputs
</commit_message>
<xml_diff>
--- a/Data/All_matched_groups_20230306_V2.xlsx
+++ b/Data/All_matched_groups_20230306_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsdha\OneDrive - 11593765 Canada Association\Fares Drive\Works in progress\RDA\RDA_Analytics\RDA_Pathways_mapping\Outputs_pdf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsdha\Desktop\New folder\RDA_Pathways\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F56E1E-38A4-4173-AD94-0C89FC589433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF169CB-BEE2-48A1-ACF5-B02A46CD300C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{D6A0B19C-0332-4BD3-B850-1BF685A0DFED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D6A0B19C-0332-4BD3-B850-1BF685A0DFED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="121">
   <si>
     <t>Blockchain Applications in Health WG</t>
   </si>
@@ -360,13 +360,52 @@
   </si>
   <si>
     <t>Psychological Data IG</t>
+  </si>
+  <si>
+    <t>FAIR, CARE, TRUST - Principles, Semantics, Ontology, Standardisation</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Training, Stewardship, and Data Management Planning,</t>
+  </si>
+  <si>
+    <t>National PID Strategies Interest Group</t>
+  </si>
+  <si>
+    <t>RDA-OfR Mapping the digital research data infrastructure landscape WG</t>
+  </si>
+  <si>
+    <t>RDA / CODATA Data Systems, Tools, and Services for Crisis Situations WG</t>
+  </si>
+  <si>
+    <t>Working with PIDs in Tools IG</t>
+  </si>
+  <si>
+    <t>Science communication for research data</t>
+  </si>
+  <si>
+    <t>Ethics and Social Aspects of Data IG</t>
+  </si>
+  <si>
+    <t>Evaluation of Research IG</t>
+  </si>
+  <si>
+    <t>CoreTrustSeal Maintenance WG</t>
+  </si>
+  <si>
+    <t>Complex Citations Working Group</t>
+  </si>
+  <si>
+    <t>RDA/WDS Scholarly Link Exchange (Scholix) WG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,16 +413,316 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -391,15 +730,206 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -711,10 +1241,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9046C30-B6F2-4A72-928C-FC4F76867AEA}">
-  <dimension ref="A1:B221"/>
+  <dimension ref="A1:B272"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A188" workbookViewId="0">
-      <selection activeCell="A200" sqref="A200"/>
+    <sheetView tabSelected="1" topLeftCell="A255" workbookViewId="0">
+      <selection activeCell="A276" sqref="A276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2490,6 +3020,414 @@
         <v>101</v>
       </c>
     </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A222" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A223" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A224" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A225" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A226" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A227" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A228" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A229" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A230" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A231" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A232" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A233" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A234" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A235" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A236" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A237" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A238" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A239" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A240" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A241" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A242" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A243" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A244" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A245" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A246" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A247" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A248" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A249" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A250" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A251" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A252" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A253" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A254" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A255" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A256" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A257" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A258" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A259" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A260" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A261" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A262" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A263" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A264" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B264" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A265" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A266" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A267" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A268" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A269" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A270" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A271" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A272" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>